<commit_message>
New version of upload_template
</commit_message>
<xml_diff>
--- a/upload_template.xlsx
+++ b/upload_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tianpan/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{01960FD0-418E-8546-A072-1D33B092E1ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{941057F5-9A30-3842-82EC-1F0D80C138CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" activeTab="5" xr2:uid="{18923CA8-A5FA-2F43-922B-9764DDA1F60E}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{18923CA8-A5FA-2F43-922B-9764DDA1F60E}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="8" r:id="rId1"/>
@@ -140,16 +140,7 @@
     <t>Changes to the data:</t>
   </si>
   <si>
-    <t xml:space="preserve">If you have notived that there is an error in one of the data values, please insert the correct values for the relevant </t>
-  </si>
-  <si>
-    <t xml:space="preserve">measurement. The correct data will automatically overwrite what has previously been added. </t>
-  </si>
-  <si>
     <t xml:space="preserve">This spreadsheet is where you can fill in the data for feeding, sweat measurements and blood measurements for </t>
-  </si>
-  <si>
-    <t>each baby</t>
   </si>
   <si>
     <r>
@@ -202,6 +193,15 @@
       </rPr>
       <t xml:space="preserve"> change the sheetnames or any of the headers otherwise the data will not be displayed correctly</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">The correct data will automatically overwrite what has previously been added. </t>
+  </si>
+  <si>
+    <t>If you have noticed that there is an error in one of the data values, please add the correct values on the relevant sheet.</t>
+  </si>
+  <si>
+    <t>each baby.</t>
   </si>
 </sst>
 </file>
@@ -423,7 +423,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -738,15 +738,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4669605B-29AF-F74E-9549-99B6FB022238}">
-  <dimension ref="A1:J36"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView zoomScale="109" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10" ht="24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="24" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
         <v>21</v>
       </c>
@@ -759,7 +759,7 @@
       <c r="H1" s="20"/>
       <c r="I1" s="20"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="20"/>
       <c r="B2" s="20"/>
       <c r="C2" s="20"/>
@@ -770,9 +770,9 @@
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C3" s="20"/>
       <c r="D3" s="20"/>
@@ -782,9 +782,9 @@
       <c r="H3" s="20"/>
       <c r="I3" s="20"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B4" s="20"/>
       <c r="C4" s="20"/>
@@ -795,7 +795,7 @@
       <c r="H4" s="20"/>
       <c r="I4" s="20"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C5" s="20"/>
       <c r="D5" s="20"/>
       <c r="E5" s="20"/>
@@ -804,12 +804,12 @@
       <c r="H5" s="20"/>
       <c r="I5" s="20"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="20" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="23" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C6" s="20"/>
       <c r="D6" s="20"/>
@@ -819,7 +819,7 @@
       <c r="H6" s="20"/>
       <c r="I6" s="20"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="20"/>
       <c r="B7" s="20"/>
       <c r="C7" s="20"/>
@@ -830,7 +830,7 @@
       <c r="H7" s="20"/>
       <c r="I7" s="20"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
         <v>23</v>
       </c>
@@ -843,9 +843,9 @@
       <c r="H8" s="20"/>
       <c r="I8" s="20"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="B9" s="20"/>
       <c r="C9" s="20"/>
@@ -856,9 +856,9 @@
       <c r="H9" s="20"/>
       <c r="I9" s="20"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B10" s="20"/>
       <c r="C10" s="20"/>
@@ -869,7 +869,7 @@
       <c r="H10" s="20"/>
       <c r="I10" s="20"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B11" s="20"/>
       <c r="C11" s="20"/>
       <c r="D11" s="20"/>
@@ -879,7 +879,7 @@
       <c r="H11" s="20"/>
       <c r="I11" s="20"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="20"/>
       <c r="B12" s="20"/>
       <c r="C12" s="20"/>
@@ -890,9 +890,9 @@
       <c r="H12" s="20"/>
       <c r="I12" s="20"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B13" s="20"/>
       <c r="C13" s="20"/>
@@ -903,7 +903,7 @@
       <c r="H13" s="20"/>
       <c r="I13" s="20"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="20"/>
       <c r="B14" s="20"/>
       <c r="C14" s="20"/>
@@ -913,270 +913,6 @@
       <c r="G14" s="20"/>
       <c r="H14" s="20"/>
       <c r="I14" s="20"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A15" s="23"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="23"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A16" s="23"/>
-      <c r="B16" s="23"/>
-      <c r="C16" s="23"/>
-      <c r="D16" s="23"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A17" s="23"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="23"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A18" s="23"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="23"/>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="23"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="23"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
-      <c r="D19" s="23"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="23"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="23"/>
-      <c r="B20" s="23"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="23"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A21" s="23"/>
-      <c r="B21" s="23"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="23"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" s="23"/>
-      <c r="B22" s="23"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="23"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A23" s="23"/>
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="23"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A24" s="23"/>
-      <c r="B24" s="23"/>
-      <c r="C24" s="23"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="23"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A25" s="23"/>
-      <c r="B25" s="23"/>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="23"/>
-      <c r="I25" s="23"/>
-      <c r="J25" s="23"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A26" s="23"/>
-      <c r="B26" s="23"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="23"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" s="23"/>
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="23"/>
-      <c r="H27" s="23"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="23"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A28" s="23"/>
-      <c r="B28" s="23"/>
-      <c r="C28" s="23"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="23"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A29" s="23"/>
-      <c r="B29" s="23"/>
-      <c r="C29" s="23"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="23"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A30" s="23"/>
-      <c r="B30" s="23"/>
-      <c r="C30" s="23"/>
-      <c r="D30" s="23"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="23"/>
-      <c r="I30" s="23"/>
-      <c r="J30" s="23"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A31" s="23"/>
-      <c r="B31" s="23"/>
-      <c r="C31" s="23"/>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="23"/>
-      <c r="J31" s="23"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A32" s="23"/>
-      <c r="B32" s="23"/>
-      <c r="C32" s="23"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="23"/>
-      <c r="I32" s="23"/>
-      <c r="J32" s="23"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33" s="23"/>
-      <c r="B33" s="23"/>
-      <c r="C33" s="23"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="23"/>
-      <c r="G33" s="23"/>
-      <c r="H33" s="23"/>
-      <c r="I33" s="23"/>
-      <c r="J33" s="23"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34" s="23"/>
-      <c r="B34" s="23"/>
-      <c r="C34" s="23"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="23"/>
-      <c r="G34" s="23"/>
-      <c r="H34" s="23"/>
-      <c r="I34" s="23"/>
-      <c r="J34" s="23"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35" s="23"/>
-      <c r="B35" s="23"/>
-      <c r="C35" s="23"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="23"/>
-      <c r="G35" s="23"/>
-      <c r="H35" s="23"/>
-      <c r="I35" s="23"/>
-      <c r="J35" s="23"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="23"/>
-      <c r="B36" s="23"/>
-      <c r="C36" s="23"/>
-      <c r="D36" s="23"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="23"/>
-      <c r="G36" s="23"/>
-      <c r="H36" s="23"/>
-      <c r="I36" s="23"/>
-      <c r="J36" s="23"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
@@ -1189,7 +925,7 @@
   <dimension ref="A1:G1048575"/>
   <sheetViews>
     <sheetView zoomScale="119" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6822,6 +6558,7 @@
       <c r="B1048575" s="6"/>
     </row>
   </sheetData>
+  <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -10707,7 +10444,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18820D39-812D-DB42-80E8-5FB1B9E4B1BF}">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>

</xml_diff>